<commit_message>
Introduced WeaponSystem.Transfers Introduced class MongoDbToMsSqlAgent. to holg tasks fot transfering the data.
</commit_message>
<xml_diff>
--- a/New folder/Manufacturers.xlsx
+++ b/New folder/Manufacturers.xlsx
@@ -22,20 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Counntry</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Česká zbrojovka</t>
   </si>
   <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
     <t>Magnum Research</t>
   </si>
   <si>
@@ -51,9 +42,6 @@
     <t>Heckler&amp;Koch</t>
   </si>
   <si>
-    <t>Germany</t>
-  </si>
-  <si>
     <t>Smith&amp;Wesson</t>
   </si>
   <si>
@@ -66,15 +54,9 @@
     <t>Benelli</t>
   </si>
   <si>
-    <t>Italy</t>
-  </si>
-  <si>
     <t>Izhmash</t>
   </si>
   <si>
-    <t>Russia</t>
-  </si>
-  <si>
     <t>MAC</t>
   </si>
   <si>
@@ -84,9 +66,6 @@
     <t>Styer</t>
   </si>
   <si>
-    <t>Austria</t>
-  </si>
-  <si>
     <t>FN Herstal</t>
   </si>
   <si>
@@ -96,18 +75,12 @@
     <t>IMI</t>
   </si>
   <si>
-    <t>Israel</t>
-  </si>
-  <si>
     <t>Barret</t>
   </si>
   <si>
     <t>Philippine Marine Corps</t>
   </si>
   <si>
-    <t>Philippines</t>
-  </si>
-  <si>
     <t>FNH USA</t>
   </si>
   <si>
@@ -117,19 +90,13 @@
     <t>Fabrique Nationale de Herstal</t>
   </si>
   <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Swaziland</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Country</t>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>CountryId</t>
   </si>
 </sst>
 </file>
@@ -483,222 +450,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.5703125"/>
-    <col min="2" max="2" width="14.5703125"/>
-    <col min="3" max="1025" width="11.5703125"/>
+    <col min="2" max="2" width="29.5703125"/>
+    <col min="3" max="3" width="14.5703125"/>
+    <col min="4" max="1026" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C20">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C21">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>32</v>
+      <c r="C24">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" tooltip="Belgium" display="https://en.wikipedia.org/wiki/Belgium"/>
+    <hyperlink ref="C19" r:id="rId1" tooltip="Belgium" display="https://en.wikipedia.org/wiki/Belgium"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId2"/>

</xml_diff>